<commit_message>
code clean up and source.xlsx is exactly the same
</commit_message>
<xml_diff>
--- a/utils/excel_files/source.xlsx
+++ b/utils/excel_files/source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\OneDrive\Desktop\MIT\cript-excel-uploader\utils\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A6F19F-99F0-4259-B586-250A83D3F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D5E948-5802-4749-B280-CE6D123E3CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
   </bookViews>
@@ -2501,7 +2501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3B6A50-1025-42AE-89F7-24E7EE793A8D}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added attributes and relation sheet to source.xlsx
</commit_message>
<xml_diff>
--- a/utils/excel_files/source.xlsx
+++ b/utils/excel_files/source.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\OneDrive\Desktop\MIT\cript-excel-uploader\utils\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D5E948-5802-4749-B280-CE6D123E3CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB92359-07FC-4990-85B0-D93989B7AAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
   </bookViews>
   <sheets>
     <sheet name="property" sheetId="1" r:id="rId1"/>
-    <sheet name="type" sheetId="2" r:id="rId2"/>
-    <sheet name="condition" sheetId="3" r:id="rId3"/>
-    <sheet name="keywords" sheetId="4" r:id="rId4"/>
-    <sheet name="identifiers" sheetId="5" r:id="rId5"/>
+    <sheet name="attribute" sheetId="6" r:id="rId2"/>
+    <sheet name="relation" sheetId="7" r:id="rId3"/>
+    <sheet name="type" sheetId="2" r:id="rId4"/>
+    <sheet name="condition" sheetId="3" r:id="rId5"/>
+    <sheet name="keywords" sheetId="4" r:id="rId6"/>
+    <sheet name="identifiers" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="690">
   <si>
     <t>Name</t>
   </si>
@@ -2077,6 +2079,39 @@
   </si>
   <si>
     <t>company the material was obtain from</t>
+  </si>
+  <si>
+    <t>uncertainty</t>
+  </si>
+  <si>
+    <t>uncertainty_type</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>structure</t>
+  </si>
+  <si>
+    <t>sample_preparation</t>
+  </si>
+  <si>
+    <t>set_id</t>
+  </si>
+  <si>
+    <t>conditions</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>citation</t>
   </si>
 </sst>
 </file>
@@ -2150,6 +2185,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{08375CC6-08AA-43D6-AB3A-756AAC89AEAC}" name="Table6" displayName="Table6" ref="A1:A10" totalsRowShown="0">
+  <autoFilter ref="A1:A10" xr:uid="{08375CC6-08AA-43D6-AB3A-756AAC89AEAC}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{63AFB5D7-0B16-4138-8D3D-3769B8DC39F9}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{EF05AA22-DDA4-4803-AD8D-33C0EB69322C}" name="Table7" displayName="Table7" ref="A1:A3" totalsRowShown="0">
+  <autoFilter ref="A1:A3" xr:uid="{EF05AA22-DDA4-4803-AD8D-33C0EB69322C}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{A16340DD-AE79-4E1F-A754-97F58F670DE9}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2DC5A8CE-6E1C-43BC-B8E8-26149E0DBD79}" name="Table3" displayName="Table3" ref="A1:B7" totalsRowShown="0">
   <autoFilter ref="A1:B7" xr:uid="{2DC5A8CE-6E1C-43BC-B8E8-26149E0DBD79}"/>
   <tableColumns count="2">
@@ -2160,7 +2215,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{425CF15F-35FC-474B-B4FD-24BB93CF909F}" name="Table4" displayName="Table4" ref="A1:H41" totalsRowShown="0">
   <autoFilter ref="A1:H41" xr:uid="{425CF15F-35FC-474B-B4FD-24BB93CF909F}"/>
   <tableColumns count="8">
@@ -2177,7 +2232,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{83C72D4E-1636-49AF-AFF3-6DAEBDE31235}" name="Table2" displayName="Table2" ref="A1:B85" totalsRowShown="0">
   <autoFilter ref="A1:B85" xr:uid="{83C72D4E-1636-49AF-AFF3-6DAEBDE31235}"/>
   <tableColumns count="2">
@@ -2188,7 +2243,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1C45AF1E-E72D-4180-AEA3-B582132E9976}" name="Table5" displayName="Table5" ref="A1:E15" totalsRowShown="0">
   <autoFilter ref="A1:E15" xr:uid="{1C45AF1E-E72D-4180-AEA3-B582132E9976}"/>
   <tableColumns count="5">
@@ -2501,7 +2556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3B6A50-1025-42AE-89F7-24E7EE793A8D}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -5373,6 +5428,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8146C182-EEE9-4906-9657-C8B006E099EC}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>688</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70F78B9-7D64-4E4F-9B7A-0DB62848DDF8}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>689</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B15FBA10-6CEA-4EFA-B0E6-FE77527D1B38}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -5450,7 +5611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E599D25-C0F6-47DA-A3A8-72CA36EC3683}">
   <dimension ref="A1:H41"/>
   <sheetViews>
@@ -6526,7 +6687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D1CDBE-C0EB-4B6C-9F42-C99DC257B084}">
   <dimension ref="A1:B85"/>
   <sheetViews>
@@ -7229,7 +7390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9ABAB8-9F16-4C85-958F-9BD932FA0E18}">
   <dimension ref="A1:E15"/>
   <sheetViews>

</xml_diff>

<commit_message>
removed sample_preparation from attributes list
</commit_message>
<xml_diff>
--- a/utils/excel_files/source.xlsx
+++ b/utils/excel_files/source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\OneDrive\Desktop\MIT\cript-excel-uploader\utils\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB92359-07FC-4990-85B0-D93989B7AAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E81FBA3-BEE3-4849-AE4C-612113D7A689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="689">
   <si>
     <t>Name</t>
   </si>
@@ -2094,9 +2094,6 @@
   </si>
   <si>
     <t>structure</t>
-  </si>
-  <si>
-    <t>sample_preparation</t>
   </si>
   <si>
     <t>set_id</t>
@@ -2118,10 +2115,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2144,13 +2149,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2185,8 +2193,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{08375CC6-08AA-43D6-AB3A-756AAC89AEAC}" name="Table6" displayName="Table6" ref="A1:A10" totalsRowShown="0">
-  <autoFilter ref="A1:A10" xr:uid="{08375CC6-08AA-43D6-AB3A-756AAC89AEAC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{08375CC6-08AA-43D6-AB3A-756AAC89AEAC}" name="Table6" displayName="Table6" ref="A1:A9" totalsRowShown="0">
+  <autoFilter ref="A1:A9" xr:uid="{08375CC6-08AA-43D6-AB3A-756AAC89AEAC}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{63AFB5D7-0B16-4138-8D3D-3769B8DC39F9}" name="Name"/>
   </tableColumns>
@@ -5429,66 +5437,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8146C182-EEE9-4906-9657-C8B006E099EC}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -5517,12 +5521,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed CAS to chemical_id and removed the description of it
</commit_message>
<xml_diff>
--- a/utils/excel_files/source.xlsx
+++ b/utils/excel_files/source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\OneDrive\Desktop\MIT\cript-excel-uploader\utils\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8855632E-AAE5-469B-896D-B33BD29E12F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304700F4-7299-4484-B826-7DF6DB067B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
   </bookViews>
   <sheets>
     <sheet name="property" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="688">
   <si>
     <t>Name</t>
   </si>
@@ -2015,12 +2015,6 @@
     <t>bigSMILES line notation</t>
   </si>
   <si>
-    <t>cas</t>
-  </si>
-  <si>
-    <t>CAS number</t>
-  </si>
-  <si>
     <t>chem_formula</t>
   </si>
   <si>
@@ -2109,6 +2103,9 @@
   </si>
   <si>
     <t>citation</t>
+  </si>
+  <si>
+    <t>chemical_id</t>
   </si>
 </sst>
 </file>
@@ -2564,7 +2561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3B6A50-1025-42AE-89F7-24E7EE793A8D}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5454,43 +5451,43 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -5519,12 +5516,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
   </sheetData>
@@ -7396,8 +7393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9ABAB8-9F16-4C85-958F-9BD932FA0E18}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7479,7 +7476,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>657</v>
+        <v>687</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -7490,13 +7487,10 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
-        <v>658</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -7508,12 +7502,12 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -7525,12 +7519,12 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -7542,12 +7536,12 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
@@ -7559,12 +7553,12 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
@@ -7576,12 +7570,12 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -7598,7 +7592,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -7610,29 +7604,29 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>670</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>671</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
         <v>672</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>673</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -7644,12 +7638,12 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -7661,7 +7655,7 @@
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>